<commit_message>
Again Change in Plan
</commit_message>
<xml_diff>
--- a/DPT_INTERVIEW_PREP1.xlsx
+++ b/DPT_INTERVIEW_PREP1.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7800" windowWidth="28800" windowHeight="12420" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="9000" windowWidth="28800" windowHeight="12420" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="10" r:id="rId1"/>
     <sheet name="CLOUD SERVICES" sheetId="3" r:id="rId2"/>
     <sheet name="7-12-2021" sheetId="19" r:id="rId3"/>
     <sheet name="13-12-21" sheetId="20" r:id="rId4"/>
-    <sheet name="Int. Prep" sheetId="21" r:id="rId5"/>
+    <sheet name="22-12-21" sheetId="22" r:id="rId5"/>
+    <sheet name="Int. Prep" sheetId="21" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="327">
   <si>
     <t>SNO</t>
   </si>
@@ -854,9 +855,6 @@
     <t>DOCKER</t>
   </si>
   <si>
-    <t>DPT VIDEOS 19[49.45], 20, 21, DCC-GIT &amp; GIT HUB</t>
-  </si>
-  <si>
     <t>KUBERNETES</t>
   </si>
   <si>
@@ -927,6 +925,81 @@
   </si>
   <si>
     <t>AWS SECURITY (VPT)</t>
+  </si>
+  <si>
+    <t>git init</t>
+  </si>
+  <si>
+    <t>git config user.name</t>
+  </si>
+  <si>
+    <t>git config user.email</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>git add .</t>
+  </si>
+  <si>
+    <t>git commit -am ""</t>
+  </si>
+  <si>
+    <t>git push</t>
+  </si>
+  <si>
+    <t>git pull</t>
+  </si>
+  <si>
+    <t>git log</t>
+  </si>
+  <si>
+    <t>git clone</t>
+  </si>
+  <si>
+    <t>git diff</t>
+  </si>
+  <si>
+    <t>git reset "" --hard</t>
+  </si>
+  <si>
+    <t>git reset "" --soft</t>
+  </si>
+  <si>
+    <t>git restore --staged</t>
+  </si>
+  <si>
+    <t>git revert</t>
+  </si>
+  <si>
+    <t>git remote add origin ""</t>
+  </si>
+  <si>
+    <t>git remote -v</t>
+  </si>
+  <si>
+    <t>git branch [LIST]</t>
+  </si>
+  <si>
+    <t>git branch "" [NEW]</t>
+  </si>
+  <si>
+    <t>git checkout ""</t>
+  </si>
+  <si>
+    <t>DPT VIDEOS 19[49.45], 20, 21, 22 [36.26]</t>
+  </si>
+  <si>
+    <t>DCC-GIT &amp; GIT HUB</t>
+  </si>
+  <si>
+    <t>DPT VIDEOS</t>
+  </si>
+  <si>
+    <t>UDEMY ANSIBLE</t>
+  </si>
+  <si>
+    <t>HAHAHA PLAN CHANGED</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1145,6 +1218,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1866,7 +1948,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="M18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="N18">
         <v>23</v>
@@ -1885,7 +1967,7 @@
         <v>72151.59</v>
       </c>
       <c r="M19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N19">
         <v>7</v>
@@ -3714,8 +3796,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59:G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3796,7 +3878,7 @@
         <v>270</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D9" s="22" t="s">
         <v>156</v>
@@ -4069,7 +4151,7 @@
       </c>
       <c r="F20" s="21"/>
       <c r="G20" s="25" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H20" t="s">
         <v>269</v>
@@ -4093,10 +4175,10 @@
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H21" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -4120,7 +4202,7 @@
         <v>222</v>
       </c>
       <c r="H22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -4128,7 +4210,7 @@
         <v>14</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C23" s="27">
         <v>50</v>
@@ -4141,10 +4223,10 @@
       </c>
       <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -4152,7 +4234,7 @@
         <v>15</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C24" s="26">
         <v>49</v>
@@ -4164,10 +4246,10 @@
         <v>137</v>
       </c>
       <c r="F24" s="21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>278</v>
+        <v>322</v>
       </c>
       <c r="H24" t="s">
         <v>223</v>
@@ -4191,10 +4273,10 @@
       </c>
       <c r="F25" s="9"/>
       <c r="G25" s="9" t="s">
-        <v>278</v>
+        <v>323</v>
       </c>
       <c r="H25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -4202,7 +4284,7 @@
         <v>17</v>
       </c>
       <c r="B26" s="28" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C26" s="2">
         <v>47</v>
@@ -4223,7 +4305,7 @@
         <v>18</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C27" s="2">
         <v>46</v>
@@ -4244,7 +4326,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C28" s="2">
         <v>45</v>
@@ -4259,6 +4341,9 @@
       <c r="G28" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="P28" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
@@ -4283,13 +4368,16 @@
       <c r="H29" t="s">
         <v>224</v>
       </c>
+      <c r="P29" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>21</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C30" s="2">
         <v>43</v>
@@ -4304,6 +4392,9 @@
       <c r="G30" s="9" t="s">
         <v>201</v>
       </c>
+      <c r="P30" t="s">
+        <v>304</v>
+      </c>
       <c r="S30" s="24"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -4320,6 +4411,9 @@
       <c r="G31" s="9" t="s">
         <v>202</v>
       </c>
+      <c r="P31" t="s">
+        <v>317</v>
+      </c>
       <c r="S31" s="24"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -4339,6 +4433,9 @@
       <c r="H32" t="s">
         <v>225</v>
       </c>
+      <c r="P32" t="s">
+        <v>318</v>
+      </c>
       <c r="S32" s="24"/>
     </row>
     <row r="33" spans="3:19" x14ac:dyDescent="0.25">
@@ -4355,6 +4452,9 @@
       <c r="G33" s="14" t="s">
         <v>203</v>
       </c>
+      <c r="P33" t="s">
+        <v>311</v>
+      </c>
       <c r="S33" s="24"/>
     </row>
     <row r="34" spans="3:19" x14ac:dyDescent="0.25">
@@ -4371,6 +4471,9 @@
       <c r="G34" s="14" t="s">
         <v>204</v>
       </c>
+      <c r="P34" t="s">
+        <v>305</v>
+      </c>
       <c r="S34" s="24"/>
     </row>
     <row r="35" spans="3:19" x14ac:dyDescent="0.25">
@@ -4387,6 +4490,9 @@
       <c r="G35" s="14" t="s">
         <v>204</v>
       </c>
+      <c r="P35" t="s">
+        <v>306</v>
+      </c>
       <c r="S35" s="24"/>
     </row>
     <row r="36" spans="3:19" x14ac:dyDescent="0.25">
@@ -4403,6 +4509,9 @@
       <c r="G36" s="14" t="s">
         <v>206</v>
       </c>
+      <c r="P36" t="s">
+        <v>307</v>
+      </c>
       <c r="S36" s="24"/>
     </row>
     <row r="37" spans="3:19" x14ac:dyDescent="0.25">
@@ -4419,6 +4528,9 @@
       <c r="G37" s="14" t="s">
         <v>207</v>
       </c>
+      <c r="P37" t="s">
+        <v>309</v>
+      </c>
       <c r="S37" s="24"/>
     </row>
     <row r="38" spans="3:19" x14ac:dyDescent="0.25">
@@ -4435,6 +4547,9 @@
       <c r="G38" s="14" t="s">
         <v>208</v>
       </c>
+      <c r="P38" t="s">
+        <v>308</v>
+      </c>
       <c r="S38" s="24"/>
     </row>
     <row r="39" spans="3:19" x14ac:dyDescent="0.25">
@@ -4451,6 +4566,9 @@
       <c r="G39" s="14" t="s">
         <v>208</v>
       </c>
+      <c r="P39" t="s">
+        <v>310</v>
+      </c>
       <c r="S39" s="24"/>
     </row>
     <row r="40" spans="3:19" x14ac:dyDescent="0.25">
@@ -4467,6 +4585,9 @@
       <c r="G40" s="14" t="s">
         <v>208</v>
       </c>
+      <c r="P40" t="s">
+        <v>312</v>
+      </c>
       <c r="S40" s="24"/>
     </row>
     <row r="41" spans="3:19" x14ac:dyDescent="0.25">
@@ -4483,6 +4604,9 @@
       <c r="G41" s="14" t="s">
         <v>208</v>
       </c>
+      <c r="P41" t="s">
+        <v>313</v>
+      </c>
       <c r="S41" s="24"/>
     </row>
     <row r="42" spans="3:19" x14ac:dyDescent="0.25">
@@ -4502,6 +4626,9 @@
       <c r="H42" t="s">
         <v>226</v>
       </c>
+      <c r="P42" t="s">
+        <v>314</v>
+      </c>
       <c r="S42" s="24"/>
     </row>
     <row r="43" spans="3:19" x14ac:dyDescent="0.25">
@@ -4518,6 +4645,9 @@
       <c r="G43" s="14" t="s">
         <v>215</v>
       </c>
+      <c r="P43" t="s">
+        <v>315</v>
+      </c>
       <c r="S43" s="24"/>
     </row>
     <row r="44" spans="3:19" x14ac:dyDescent="0.25">
@@ -4534,6 +4664,9 @@
       <c r="G44" s="14" t="s">
         <v>215</v>
       </c>
+      <c r="P44" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
@@ -4552,6 +4685,9 @@
       <c r="H45" t="s">
         <v>227</v>
       </c>
+      <c r="P45" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="46" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
@@ -4567,6 +4703,9 @@
       <c r="G46" s="9" t="s">
         <v>210</v>
       </c>
+      <c r="P46" t="s">
+        <v>320</v>
+      </c>
     </row>
     <row r="47" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
@@ -4582,6 +4721,9 @@
       <c r="G47" s="9" t="s">
         <v>211</v>
       </c>
+      <c r="P47" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
@@ -4844,7 +4986,7 @@
         <v>246</v>
       </c>
       <c r="H64" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
@@ -4862,7 +5004,7 @@
         <v>218</v>
       </c>
       <c r="H65" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -4880,7 +5022,7 @@
         <v>218</v>
       </c>
       <c r="H66" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.25">
@@ -4987,6 +5129,1217 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>184</v>
+      </c>
+      <c r="M2" s="9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>185</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>186</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>187</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>188</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q6" s="24" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>190</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="M8" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>285</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>1</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>271</v>
+      </c>
+      <c r="C10" s="26">
+        <v>63</v>
+      </c>
+      <c r="D10" s="20">
+        <v>44537</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>2</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="C11" s="26">
+        <v>62</v>
+      </c>
+      <c r="D11" s="20">
+        <v>44538</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="H11" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>3</v>
+      </c>
+      <c r="B12" s="21" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" s="26">
+        <v>61</v>
+      </c>
+      <c r="D12" s="20">
+        <v>44539</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="H12" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>4</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="26">
+        <v>60</v>
+      </c>
+      <c r="D13" s="20">
+        <v>44540</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
+        <v>231</v>
+      </c>
+      <c r="H13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>5</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="C14" s="26">
+        <v>59</v>
+      </c>
+      <c r="D14" s="20">
+        <v>44541</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="H14" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>6</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>275</v>
+      </c>
+      <c r="C15" s="27">
+        <v>58</v>
+      </c>
+      <c r="D15" s="18">
+        <v>44542</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19" t="s">
+        <v>234</v>
+      </c>
+      <c r="H15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>7</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="27">
+        <v>57</v>
+      </c>
+      <c r="D16" s="18">
+        <v>44543</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19" t="s">
+        <v>245</v>
+      </c>
+      <c r="H16" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>8</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="26">
+        <v>56</v>
+      </c>
+      <c r="D17" s="20">
+        <v>44544</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F17" s="21"/>
+      <c r="G17" s="23" t="s">
+        <v>249</v>
+      </c>
+      <c r="H17" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>9</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" s="26">
+        <v>55</v>
+      </c>
+      <c r="D18" s="20">
+        <v>44545</v>
+      </c>
+      <c r="E18" s="21" t="s">
+        <v>138</v>
+      </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21" t="s">
+        <v>250</v>
+      </c>
+      <c r="H18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>10</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C19" s="26">
+        <v>54</v>
+      </c>
+      <c r="D19" s="20">
+        <v>44546</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="H19" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>11</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="26">
+        <v>53</v>
+      </c>
+      <c r="D20" s="20">
+        <v>44547</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="25" t="s">
+        <v>283</v>
+      </c>
+      <c r="H20" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>12</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="C21" s="27">
+        <v>52</v>
+      </c>
+      <c r="D21" s="18">
+        <v>44548</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>286</v>
+      </c>
+      <c r="H21" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>13</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C22" s="27">
+        <v>51</v>
+      </c>
+      <c r="D22" s="18">
+        <v>44549</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="H22" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>14</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="C23" s="27">
+        <v>50</v>
+      </c>
+      <c r="D23" s="18">
+        <v>44550</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="H23" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>15</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="C24" s="26">
+        <v>49</v>
+      </c>
+      <c r="D24" s="20">
+        <v>44551</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>301</v>
+      </c>
+      <c r="G24" s="21" t="s">
+        <v>322</v>
+      </c>
+      <c r="H24" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>16</v>
+      </c>
+      <c r="B25" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="C25" s="29">
+        <v>48</v>
+      </c>
+      <c r="D25" s="30">
+        <v>44552</v>
+      </c>
+      <c r="E25" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="H25" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>17</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>300</v>
+      </c>
+      <c r="C26" s="2">
+        <v>47</v>
+      </c>
+      <c r="D26" s="13">
+        <v>44553</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>18</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="C27" s="2">
+        <v>46</v>
+      </c>
+      <c r="D27" s="13">
+        <v>44554</v>
+      </c>
+      <c r="E27" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>19</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="C28" s="2">
+        <v>45</v>
+      </c>
+      <c r="D28" s="13">
+        <v>44555</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>20</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44</v>
+      </c>
+      <c r="D29" s="13">
+        <v>44556</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H29" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>21</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="2">
+        <v>43</v>
+      </c>
+      <c r="D30" s="13">
+        <v>44557</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="S30" s="24"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <v>42</v>
+      </c>
+      <c r="D31" s="13">
+        <v>44558</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="S31" s="24"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <v>41</v>
+      </c>
+      <c r="D32" s="13">
+        <v>44559</v>
+      </c>
+      <c r="E32" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="H32" t="s">
+        <v>225</v>
+      </c>
+      <c r="S32" s="24"/>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <v>40</v>
+      </c>
+      <c r="D33" s="13">
+        <v>44560</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="S33" s="24"/>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <v>39</v>
+      </c>
+      <c r="D34" s="13">
+        <v>44561</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="S34" s="24"/>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <v>38</v>
+      </c>
+      <c r="D35" s="13">
+        <v>44562</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F35" s="9"/>
+      <c r="G35" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="S35" s="24"/>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <v>37</v>
+      </c>
+      <c r="D36" s="13">
+        <v>44563</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F36" s="9"/>
+      <c r="G36" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="S36" s="24"/>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <v>36</v>
+      </c>
+      <c r="D37" s="13">
+        <v>44564</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="S37" s="24"/>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <v>35</v>
+      </c>
+      <c r="D38" s="13">
+        <v>44565</v>
+      </c>
+      <c r="E38" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="S38" s="24"/>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <v>34</v>
+      </c>
+      <c r="D39" s="13">
+        <v>44566</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="S39" s="24"/>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <v>33</v>
+      </c>
+      <c r="D40" s="13">
+        <v>44567</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="S40" s="24"/>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <v>32</v>
+      </c>
+      <c r="D41" s="13">
+        <v>44568</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="S41" s="24"/>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <v>31</v>
+      </c>
+      <c r="D42" s="13">
+        <v>44569</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="H42" t="s">
+        <v>226</v>
+      </c>
+      <c r="S42" s="24"/>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <v>30</v>
+      </c>
+      <c r="D43" s="13">
+        <v>44570</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F43" s="9"/>
+      <c r="G43" s="14"/>
+      <c r="S43" s="24"/>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <v>29</v>
+      </c>
+      <c r="D44" s="13">
+        <v>44571</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F44" s="9"/>
+      <c r="G44" s="14"/>
+    </row>
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <v>28</v>
+      </c>
+      <c r="D45" s="13">
+        <v>44572</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F45" s="9"/>
+      <c r="G45" s="14"/>
+      <c r="H45" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <v>27</v>
+      </c>
+      <c r="D46" s="13">
+        <v>44573</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F46" s="9"/>
+      <c r="G46" s="9"/>
+    </row>
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <v>26</v>
+      </c>
+      <c r="D47" s="13">
+        <v>44574</v>
+      </c>
+      <c r="E47" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F47" s="9"/>
+      <c r="G47" s="9"/>
+    </row>
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <v>25</v>
+      </c>
+      <c r="D48" s="13">
+        <v>44575</v>
+      </c>
+      <c r="E48" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F48" s="9"/>
+      <c r="G48" s="9"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <v>24</v>
+      </c>
+      <c r="D49" s="13">
+        <v>44576</v>
+      </c>
+      <c r="E49" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F49" s="9"/>
+      <c r="G49" s="9"/>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <v>23</v>
+      </c>
+      <c r="D50" s="13">
+        <v>44577</v>
+      </c>
+      <c r="E50" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F50" s="9"/>
+      <c r="G50" s="9"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <v>22</v>
+      </c>
+      <c r="D51" s="13">
+        <v>44578</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <v>21</v>
+      </c>
+      <c r="D52" s="13">
+        <v>44579</v>
+      </c>
+      <c r="E52" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F52" s="9"/>
+      <c r="G52" s="9"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <v>20</v>
+      </c>
+      <c r="D53" s="13">
+        <v>44580</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F53" s="9"/>
+      <c r="G53" s="9"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <v>19</v>
+      </c>
+      <c r="D54" s="13">
+        <v>44581</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
+      <c r="H54" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <v>18</v>
+      </c>
+      <c r="D55" s="13">
+        <v>44582</v>
+      </c>
+      <c r="E55" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F55" s="9"/>
+      <c r="G55" s="9"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="2">
+        <v>17</v>
+      </c>
+      <c r="D56" s="13">
+        <v>44583</v>
+      </c>
+      <c r="E56" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F56" s="9"/>
+      <c r="G56" s="9"/>
+      <c r="H56" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="2">
+        <v>16</v>
+      </c>
+      <c r="D57" s="13">
+        <v>44584</v>
+      </c>
+      <c r="E57" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F57" s="9"/>
+      <c r="G57" s="9"/>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="2">
+        <v>15</v>
+      </c>
+      <c r="D58" s="13">
+        <v>44585</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" s="9"/>
+      <c r="G58" s="9"/>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="2">
+        <v>14</v>
+      </c>
+      <c r="D59" s="13">
+        <v>44586</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F59" s="9"/>
+      <c r="G59" s="9"/>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="2">
+        <v>13</v>
+      </c>
+      <c r="D60" s="13">
+        <v>44587</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F60" s="9"/>
+      <c r="G60" s="9"/>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="2">
+        <v>12</v>
+      </c>
+      <c r="D61" s="13">
+        <v>44588</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F61" s="9"/>
+      <c r="G61" s="9"/>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="2">
+        <v>11</v>
+      </c>
+      <c r="D62" s="13">
+        <v>44589</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F62" s="9"/>
+      <c r="G62" s="9"/>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="2">
+        <v>10</v>
+      </c>
+      <c r="D63" s="13">
+        <v>44590</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F63" s="9"/>
+      <c r="G63" s="9"/>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="2">
+        <v>9</v>
+      </c>
+      <c r="D64" s="13">
+        <v>44591</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F64" s="9"/>
+      <c r="G64" s="9"/>
+      <c r="H64" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="2">
+        <v>8</v>
+      </c>
+      <c r="D65" s="13">
+        <v>44592</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F65" s="9"/>
+      <c r="G65" s="9"/>
+      <c r="H65" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="2">
+        <v>7</v>
+      </c>
+      <c r="D66" s="13">
+        <v>44593</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F66" s="9"/>
+      <c r="G66" s="9"/>
+      <c r="H66" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="2">
+        <v>6</v>
+      </c>
+      <c r="D67" s="13">
+        <v>44594</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F67" s="9"/>
+      <c r="G67" s="9"/>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="2">
+        <v>5</v>
+      </c>
+      <c r="D68" s="13">
+        <v>44595</v>
+      </c>
+      <c r="E68" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F68" s="9"/>
+      <c r="G68" s="9"/>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="2">
+        <v>4</v>
+      </c>
+      <c r="D69" s="13">
+        <v>44596</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F69" s="9"/>
+      <c r="G69" s="9"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="2">
+        <v>3</v>
+      </c>
+      <c r="D70" s="13">
+        <v>44597</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="F70" s="9"/>
+      <c r="G70" s="9"/>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="2">
+        <v>2</v>
+      </c>
+      <c r="D71" s="13">
+        <v>44598</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="F71" s="9"/>
+      <c r="G71" s="9"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="2">
+        <v>1</v>
+      </c>
+      <c r="D72" s="13">
+        <v>44599</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F72" s="9"/>
+      <c r="G72" s="9"/>
+      <c r="H72" t="s">
+        <v>230</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4997,27 +6350,27 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>

</xml_diff>